<commit_message>
- Add Tam ung
</commit_message>
<xml_diff>
--- a/document/Task_Planning.xlsx
+++ b/document/Task_Planning.xlsx
@@ -181,7 +181,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,6 +230,12 @@
     <font>
       <sz val="11"/>
       <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -325,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -400,7 +406,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1103,10 +1113,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1119,7 +1129,7 @@
     <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
         <v>38</v>
       </c>
@@ -1130,12 +1140,12 @@
       <c r="F1" s="30"/>
       <c r="G1" s="30"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G2" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
@@ -1157,8 +1167,9 @@
       <c r="G3" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J3" s="36"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="17"/>
       <c r="B4" s="19" t="s">
         <v>26</v>
@@ -1175,7 +1186,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="17"/>
       <c r="B5" s="10"/>
       <c r="C5" s="24" t="s">
@@ -1188,10 +1199,10 @@
       <c r="F5" s="1"/>
       <c r="G5" s="32"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="18"/>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="34" t="s">
         <v>27</v>
       </c>
       <c r="D6" s="1"/>
@@ -1201,7 +1212,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="32"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="17"/>
       <c r="B7" s="18"/>
       <c r="C7" s="23" t="s">
@@ -1214,7 +1225,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="33"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="17"/>
       <c r="B8" s="10" t="s">
         <v>28</v>
@@ -1227,7 +1238,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" s="18"/>
       <c r="C9" s="4" t="s">
@@ -1238,7 +1249,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
       <c r="B10" s="11" t="s">
         <v>37</v>
@@ -1246,14 +1257,14 @@
       <c r="C10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="D10" s="35" t="s">
         <v>40</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="23"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
       <c r="B11" s="16"/>
       <c r="C11" s="4"/>
@@ -1264,7 +1275,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="23"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
       <c r="B12" s="16" t="s">
         <v>0</v>
@@ -1277,7 +1288,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="17"/>
       <c r="B13" s="19"/>
       <c r="C13" s="21" t="s">
@@ -1288,7 +1299,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="17"/>
       <c r="B14" s="10" t="s">
         <v>28</v>
@@ -1299,7 +1310,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="18"/>
       <c r="C15" s="1" t="s">
@@ -1312,11 +1323,11 @@
         <v>46</v>
       </c>
       <c r="F15" s="1"/>
-      <c r="G15" s="23" t="s">
+      <c r="G15" s="35" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="5"/>
       <c r="D16" t="s">

</xml_diff>

<commit_message>
- Tam ung list
</commit_message>
<xml_diff>
--- a/document/Task_Planning.xlsx
+++ b/document/Task_Planning.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="51">
   <si>
     <t>Accounting</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>24,25</t>
+  </si>
+  <si>
+    <t>Tam ung workflow</t>
   </si>
 </sst>
 </file>
@@ -331,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -411,6 +414,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1116,7 +1120,7 @@
   <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1174,13 +1178,11 @@
       <c r="B4" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="24" t="s">
-        <v>24</v>
+      <c r="C4" s="37" t="s">
+        <v>50</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="1" t="s">
-        <v>44</v>
-      </c>
+      <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="31" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
- Tam ung & Phieu chi
</commit_message>
<xml_diff>
--- a/document/Task_Planning.xlsx
+++ b/document/Task_Planning.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="50">
   <si>
     <t>Accounting</t>
   </si>
@@ -175,16 +175,13 @@
   </si>
   <si>
     <t>24,25</t>
-  </si>
-  <si>
-    <t>Tam ung workflow</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,6 +236,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -385,7 +389,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -415,6 +418,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -712,16 +716,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G2" s="2" t="s">
@@ -862,7 +866,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="27">
+      <c r="H9" s="26">
         <v>250</v>
       </c>
     </row>
@@ -876,7 +880,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="28"/>
+      <c r="H10" s="27"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
@@ -888,7 +892,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="29"/>
+      <c r="H11" s="28"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="17">
@@ -926,7 +930,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="27">
+      <c r="H13" s="26">
         <v>500</v>
       </c>
     </row>
@@ -940,7 +944,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="28"/>
+      <c r="H14" s="27"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
@@ -952,7 +956,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="28"/>
+      <c r="H15" s="27"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
@@ -964,7 +968,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="29"/>
+      <c r="H16" s="28"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="20">
@@ -1120,7 +1124,7 @@
   <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1134,15 +1138,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G2" s="2" t="s">
@@ -1171,27 +1175,25 @@
       <c r="G3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="36"/>
+      <c r="J3" s="35"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="17"/>
       <c r="B4" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="37" t="s">
-        <v>50</v>
-      </c>
+      <c r="C4" s="36"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="31" t="s">
+      <c r="G4" s="30" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="17"/>
       <c r="B5" s="10"/>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="36" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="1"/>
@@ -1199,12 +1201,12 @@
         <v>44</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="32"/>
+      <c r="G5" s="31"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="18"/>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="33" t="s">
         <v>27</v>
       </c>
       <c r="D6" s="1"/>
@@ -1212,7 +1214,7 @@
         <v>44</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="32"/>
+      <c r="G6" s="31"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="17"/>
@@ -1225,14 +1227,14 @@
         <v>44</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="33"/>
+      <c r="G7" s="32"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="17"/>
       <c r="B8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="25" t="s">
         <v>29</v>
       </c>
       <c r="D8" s="1"/>
@@ -1256,10 +1258,10 @@
       <c r="B10" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="35" t="s">
+      <c r="D10" s="34" t="s">
         <v>40</v>
       </c>
       <c r="E10" s="1"/>
@@ -1270,7 +1272,7 @@
       <c r="A11" s="17"/>
       <c r="B11" s="16"/>
       <c r="C11" s="4"/>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="37" t="s">
         <v>41</v>
       </c>
       <c r="E11" s="1"/>
@@ -1282,7 +1284,7 @@
       <c r="B12" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="24" t="s">
         <v>12</v>
       </c>
       <c r="D12" s="1"/>
@@ -1325,7 +1327,7 @@
         <v>46</v>
       </c>
       <c r="F15" s="1"/>
-      <c r="G15" s="35" t="s">
+      <c r="G15" s="34" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- Update task planing - Fixe bug: seal no
</commit_message>
<xml_diff>
--- a/document/Task_Planning.xlsx
+++ b/document/Task_Planning.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="51">
   <si>
     <t>Accounting</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Dịch vụ thông quan (chi tiết)</t>
   </si>
   <si>
-    <t>Export excel</t>
-  </si>
-  <si>
     <t>Dealine</t>
   </si>
   <si>
@@ -67,12 +64,6 @@
     <t>Profit load</t>
   </si>
   <si>
-    <t>Export Excel</t>
-  </si>
-  <si>
-    <t>Export PDF</t>
-  </si>
-  <si>
     <t>Price</t>
   </si>
   <si>
@@ -118,9 +109,6 @@
     <t>Shipment control</t>
   </si>
   <si>
-    <t>13/3</t>
-  </si>
-  <si>
     <t>Kế hoạch vận tải</t>
   </si>
   <si>
@@ -133,18 +121,9 @@
     <t>Tasks Tracking</t>
   </si>
   <si>
-    <t>Importing</t>
-  </si>
-  <si>
     <t>Done</t>
   </si>
   <si>
-    <t>Filter</t>
-  </si>
-  <si>
-    <t>UI restructure</t>
-  </si>
-  <si>
     <t>Tasks Tracking (Phuc)</t>
   </si>
   <si>
@@ -154,13 +133,52 @@
     <t>27/3</t>
   </si>
   <si>
-    <t>29/3</t>
-  </si>
-  <si>
     <t>28/3</t>
   </si>
   <si>
     <t>30/3</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Page/Function</t>
+  </si>
+  <si>
+    <t>Filters</t>
+  </si>
+  <si>
+    <t>UI decoration</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Nếu ngày hiệu lực ko nhập thì chọn ngày mặc định</t>
+  </si>
+  <si>
+    <t>Default chỉ hiện các job chưa xử lý</t>
+  </si>
+  <si>
+    <t>Manifest</t>
+  </si>
+  <si>
+    <t>FCL/LCL</t>
+  </si>
+  <si>
+    <t>Khi chuyển đổi -&gt; ảnh hưởng trucking</t>
+  </si>
+  <si>
+    <t>JS tính tổng tiền tạm ứng</t>
+  </si>
+  <si>
+    <t>Load tồn tạm ứng</t>
+  </si>
+  <si>
+    <t>Thêm time dự kiến hoàn ứng</t>
+  </si>
+  <si>
+    <t>Lưu total fee for all</t>
   </si>
 </sst>
 </file>
@@ -380,15 +398,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -401,7 +411,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -682,10 +696,394 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="16">
+        <v>1</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="30"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="30"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="30"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="30"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="30"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="16">
+        <v>2</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="16"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="16">
+        <v>3</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="30"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="16">
+        <v>4</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="29"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="16"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="29"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="29"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="9"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="29"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="19">
+        <v>5</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="29"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="29"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="29">
+        <v>42097</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="29">
+        <v>42097</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="9"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="29">
+        <v>42097</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="5"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="5"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="5"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="5"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="5"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="5"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="5"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="5"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
+      <c r="B30" s="5"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="5"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="5"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
+      <c r="B33" s="5"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="6"/>
+      <c r="B34" s="5"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="6"/>
+      <c r="B35" s="5"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="5"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="6"/>
+      <c r="B37" s="5"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="6"/>
+      <c r="B38" s="5"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
+      <c r="B39" s="5"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="5"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,29 +1097,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="A1" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G2" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H2">
-        <f>SUM(H4:H40)</f>
-        <v>2200</v>
+        <f>SUM(H4:H20)</f>
+        <v>1450</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>2</v>
@@ -733,16 +1131,16 @@
         <v>4</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>1</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -752,452 +1150,14 @@
       <c r="B4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" s="1">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="H5" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="13" t="s">
+      <c r="C4" s="31" t="s">
         <v>11</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="H6" s="1">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" s="1">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" s="1">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="16">
-        <v>2</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="31">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="32"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="33"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="16">
-        <v>3</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" s="4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="16">
-        <v>4</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="29">
-        <v>42097</v>
-      </c>
-      <c r="H13" s="31">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="29">
-        <v>42097</v>
-      </c>
-      <c r="H14" s="32"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="29">
-        <v>42097</v>
-      </c>
-      <c r="H15" s="32"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="29">
-        <v>42097</v>
-      </c>
-      <c r="H16" s="33"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="19">
-        <v>5</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="29">
-        <v>42095</v>
-      </c>
-      <c r="H17" s="1">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="29">
-        <v>42095</v>
-      </c>
-      <c r="H18" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="5"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="5"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="5"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="5"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="5"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="5"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="5"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="5"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="5"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="5"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="5"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="B30" s="5"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="5"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="B32" s="5"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="5"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="5"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-      <c r="B35" s="5"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="5"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="5"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="5"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" s="5"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="H9:H11"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="H13:H16"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H35"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2">
-        <f>SUM(H4:H20)</f>
-        <v>1450</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="16">
-        <v>1</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="38" t="s">
-        <v>12</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="3"/>
       <c r="G4" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="H4" s="1">
         <v>500</v>
@@ -1207,13 +1167,13 @@
       <c r="A5" s="16"/>
       <c r="B5" s="14"/>
       <c r="C5" s="20" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H5" s="1">
         <v>150</v>
@@ -1223,15 +1183,15 @@
       <c r="A6" s="9"/>
       <c r="B6" s="10"/>
       <c r="C6" s="22" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="H6" s="1">
         <v>500</v>
@@ -1241,13 +1201,13 @@
       <c r="A7" s="19"/>
       <c r="B7" s="17"/>
       <c r="C7" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H7" s="1">
         <v>150</v>
@@ -1258,24 +1218,31 @@
         <v>2</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H8" s="13">
         <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="5"/>
+      <c r="A9" s="6">
+        <v>3</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
@@ -1389,136 +1356,162 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:G7"/>
+      <selection activeCell="C13" activeCellId="2" sqref="C11 C12 C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" customWidth="1"/>
+    <col min="4" max="4" width="45.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
+      <c r="A1" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G2" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>1</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J3" s="26"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="18"/>
+      <c r="A4" s="16">
+        <v>1</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>37</v>
+      </c>
       <c r="C4" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="1"/>
+        <v>39</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="35"/>
+      <c r="G4" s="33"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="10"/>
-      <c r="C5" t="s">
-        <v>37</v>
+      <c r="C5" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="36"/>
+      <c r="G5" s="34"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
-      <c r="B6" s="17"/>
-      <c r="C6" t="s">
-        <v>38</v>
-      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="36"/>
+      <c r="G6" s="34"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="1"/>
+      <c r="A7" s="16">
+        <v>2</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="37"/>
+      <c r="G7" s="34"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="24"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="22"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="G8" s="35"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="1"/>
+      <c r="A9" s="16">
+        <v>3</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="25"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="22"/>
+      <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="28"/>
+      <c r="A11" s="16">
+        <v>4</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="25"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="22"/>
@@ -1526,16 +1519,20 @@
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
       <c r="B12" s="15"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="1"/>
+      <c r="C12" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="28"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="G12" s="22"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="20"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="23" t="s">
+        <v>49</v>
+      </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -1543,25 +1540,30 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="16"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="21"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="20"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="1"/>
+      <c r="A15" s="16"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="21"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="25"/>
+      <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="5"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="25"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
@@ -1644,7 +1646,7 @@
       <c r="B36" s="5"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
+      <c r="A37" s="6"/>
       <c r="B37" s="5"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1661,14 +1663,18 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="G4:G7"/>
+    <mergeCell ref="G4:G8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
- Fixed bug for release 6/4
</commit_message>
<xml_diff>
--- a/document/Task_Planning.xlsx
+++ b/document/Task_Planning.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="58">
   <si>
     <t>Accounting</t>
   </si>
@@ -197,6 +197,9 @@
   </si>
   <si>
     <t>All nescessary page</t>
+  </si>
+  <si>
+    <t>Vietnamese for all English terms</t>
   </si>
 </sst>
 </file>
@@ -290,7 +293,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -350,11 +353,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -417,10 +442,23 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -429,19 +467,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -725,7 +756,7 @@
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="C20" sqref="C20:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,15 +770,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G2" s="2"/>
@@ -778,7 +809,7 @@
       <c r="G3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="39" t="s">
+      <c r="H3" s="32" t="s">
         <v>12</v>
       </c>
     </row>
@@ -880,7 +911,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="36">
+      <c r="H9" s="35">
         <v>250</v>
       </c>
     </row>
@@ -894,7 +925,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="37"/>
+      <c r="H10" s="36"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
@@ -906,7 +937,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="38"/>
+      <c r="H11" s="37"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
@@ -942,7 +973,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="29"/>
-      <c r="H13" s="36">
+      <c r="H13" s="35">
         <v>500</v>
       </c>
     </row>
@@ -956,7 +987,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="29"/>
-      <c r="H14" s="37"/>
+      <c r="H14" s="36"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
@@ -968,7 +999,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="29"/>
-      <c r="H15" s="37"/>
+      <c r="H15" s="36"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
@@ -980,7 +1011,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="29"/>
-      <c r="H16" s="38"/>
+      <c r="H16" s="37"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
@@ -1152,30 +1183,30 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G2" s="2" t="s">
@@ -1183,7 +1214,7 @@
       </c>
       <c r="H2">
         <f>SUM(H4:H20)</f>
-        <v>1700</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1316,17 +1347,41 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="40">
+      <c r="H9" s="33">
         <v>250</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="5"/>
+      <c r="A10" s="41">
+        <v>4</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="33">
+        <v>500</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="5"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="44">
+        <v>100</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
@@ -1449,15 +1504,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G2" s="2" t="s">
@@ -1503,7 +1558,7 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="33"/>
+      <c r="G4" s="38"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
@@ -1514,7 +1569,7 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="34"/>
+      <c r="G5" s="39"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
@@ -1523,7 +1578,7 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="34"/>
+      <c r="G6" s="39"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
@@ -1540,7 +1595,7 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="34"/>
+      <c r="G7" s="39"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
@@ -1549,7 +1604,7 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="35"/>
+      <c r="G8" s="40"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="16">

</xml_diff>

<commit_message>
- Add filter for MANIFEST
</commit_message>
<xml_diff>
--- a/document/Task_Planning.xlsx
+++ b/document/Task_Planning.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="58">
   <si>
     <t>Accounting</t>
   </si>
@@ -197,6 +197,9 @@
   </si>
   <si>
     <t>All nescessary page</t>
+  </si>
+  <si>
+    <t>Vietnamese for all English terms</t>
   </si>
 </sst>
 </file>
@@ -290,7 +293,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -350,11 +353,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -417,10 +442,23 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -429,19 +467,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -725,7 +756,7 @@
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="C20" sqref="C20:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,15 +770,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G2" s="2"/>
@@ -778,7 +809,7 @@
       <c r="G3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="39" t="s">
+      <c r="H3" s="32" t="s">
         <v>12</v>
       </c>
     </row>
@@ -880,7 +911,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="36">
+      <c r="H9" s="35">
         <v>250</v>
       </c>
     </row>
@@ -894,7 +925,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="37"/>
+      <c r="H10" s="36"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
@@ -906,7 +937,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="38"/>
+      <c r="H11" s="37"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
@@ -942,7 +973,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="29"/>
-      <c r="H13" s="36">
+      <c r="H13" s="35">
         <v>500</v>
       </c>
     </row>
@@ -956,7 +987,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="29"/>
-      <c r="H14" s="37"/>
+      <c r="H14" s="36"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
@@ -968,7 +999,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="29"/>
-      <c r="H15" s="37"/>
+      <c r="H15" s="36"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
@@ -980,7 +1011,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="29"/>
-      <c r="H16" s="38"/>
+      <c r="H16" s="37"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
@@ -1152,30 +1183,30 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G2" s="2" t="s">
@@ -1183,7 +1214,7 @@
       </c>
       <c r="H2">
         <f>SUM(H4:H20)</f>
-        <v>1700</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1316,17 +1347,41 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="40">
+      <c r="H9" s="33">
         <v>250</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="5"/>
+      <c r="A10" s="41">
+        <v>4</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="33">
+        <v>500</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="5"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="44">
+        <v>100</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
@@ -1449,15 +1504,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G2" s="2" t="s">
@@ -1503,7 +1558,7 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="33"/>
+      <c r="G4" s="38"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
@@ -1514,7 +1569,7 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="34"/>
+      <c r="G5" s="39"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
@@ -1523,7 +1578,7 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="34"/>
+      <c r="G6" s="39"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
@@ -1540,7 +1595,7 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="34"/>
+      <c r="G7" s="39"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
@@ -1549,7 +1604,7 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="35"/>
+      <c r="G8" s="40"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="16">

</xml_diff>

<commit_message>
- Fixed bug: loai hang
</commit_message>
<xml_diff>
--- a/document/Task_Planning.xlsx
+++ b/document/Task_Planning.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Hien" sheetId="1" r:id="rId1"/>
     <sheet name="Phuc" sheetId="7" r:id="rId2"/>
     <sheet name="Pending" sheetId="6" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" calcMode="manual"/>
+  <calcPr calcId="152511" calcMode="manual" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="54">
   <si>
     <t>Accounting</t>
   </si>
@@ -130,15 +130,6 @@
     <t>3 sheet</t>
   </si>
   <si>
-    <t>27/3</t>
-  </si>
-  <si>
-    <t>28/3</t>
-  </si>
-  <si>
-    <t>30/3</t>
-  </si>
-  <si>
     <t>General</t>
   </si>
   <si>
@@ -173,9 +164,6 @@
   </si>
   <si>
     <t>Load tồn tạm ứng</t>
-  </si>
-  <si>
-    <t>Thêm time dự kiến hoàn ứng</t>
   </si>
   <si>
     <t>Export excel</t>
@@ -379,7 +367,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -446,33 +434,36 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -753,10 +744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20:H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,21 +761,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G2" s="2"/>
       <c r="H2">
-        <f>SUM(H4:H42)</f>
-        <v>2750</v>
+        <f>SUM(H4:H41)</f>
+        <v>2350</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -824,11 +815,13 @@
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="30"/>
+      <c r="G4" s="45">
+        <v>42102</v>
+      </c>
       <c r="H4" s="1">
         <v>150</v>
       </c>
@@ -840,11 +833,13 @@
         <v>9</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="30"/>
+      <c r="G5" s="45">
+        <v>42102</v>
+      </c>
       <c r="H5" s="1">
         <v>100</v>
       </c>
@@ -856,11 +851,13 @@
         <v>10</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="30"/>
+      <c r="G6" s="45">
+        <v>42102</v>
+      </c>
       <c r="H6" s="1">
         <v>250</v>
       </c>
@@ -872,11 +869,13 @@
         <v>11</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="30"/>
+      <c r="G7" s="45">
+        <v>42105</v>
+      </c>
       <c r="H7" s="1">
         <v>300</v>
       </c>
@@ -888,11 +887,13 @@
         <v>18</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="30"/>
+      <c r="G8" s="45">
+        <v>42103</v>
+      </c>
       <c r="H8" s="1">
         <v>150</v>
       </c>
@@ -911,7 +912,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="35">
+      <c r="H9" s="39">
         <v>250</v>
       </c>
     </row>
@@ -925,7 +926,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="36"/>
+      <c r="H10" s="40"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
@@ -937,7 +938,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="37"/>
+      <c r="H11" s="41"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
@@ -973,7 +974,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="29"/>
-      <c r="H13" s="35">
+      <c r="H13" s="39">
         <v>500</v>
       </c>
     </row>
@@ -987,7 +988,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="29"/>
-      <c r="H14" s="36"/>
+      <c r="H14" s="40"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
@@ -999,7 +1000,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="29"/>
-      <c r="H15" s="36"/>
+      <c r="H15" s="40"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
@@ -1011,7 +1012,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="29"/>
-      <c r="H16" s="37"/>
+      <c r="H16" s="41"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
@@ -1026,7 +1027,9 @@
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="29"/>
+      <c r="G17" s="29">
+        <v>42106</v>
+      </c>
       <c r="H17" s="1">
         <v>300</v>
       </c>
@@ -1040,7 +1043,9 @@
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="29"/>
+      <c r="G18" s="29">
+        <v>42103</v>
+      </c>
       <c r="H18" s="1">
         <v>100</v>
       </c>
@@ -1049,10 +1054,10 @@
       <c r="A19" s="9"/>
       <c r="B19" s="17"/>
       <c r="C19" s="25" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -1062,20 +1067,8 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="4">
-        <v>400</v>
-      </c>
+      <c r="A20" s="6"/>
+      <c r="B20" s="5"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
@@ -1142,7 +1135,7 @@
       <c r="B36" s="5"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
+      <c r="A37" s="5"/>
       <c r="B37" s="5"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1159,13 +1152,9 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1182,8 +1171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1197,16 +1186,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G2" s="2" t="s">
@@ -1256,8 +1245,8 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="1" t="s">
-        <v>34</v>
+      <c r="G4" s="29">
+        <v>42104</v>
       </c>
       <c r="H4" s="1">
         <v>500</v>
@@ -1272,8 +1261,8 @@
       <c r="D5" s="4"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1" t="s">
-        <v>35</v>
+      <c r="G5" s="29">
+        <v>42102</v>
       </c>
       <c r="H5" s="1">
         <v>150</v>
@@ -1290,9 +1279,7 @@
         <v>33</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="G6" s="1"/>
       <c r="H6" s="1">
         <v>500</v>
       </c>
@@ -1306,9 +1293,7 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="G7" s="1"/>
       <c r="H7" s="1">
         <v>150</v>
       </c>
@@ -1326,9 +1311,7 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="G8" s="1"/>
       <c r="H8" s="13">
         <v>150</v>
       </c>
@@ -1338,10 +1321,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1352,14 +1335,14 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="41">
+      <c r="A10" s="34">
         <v>4</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1372,14 +1355,14 @@
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="17"/>
-      <c r="C11" s="42" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="44">
+      <c r="C11" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="37">
         <v>100</v>
       </c>
     </row>
@@ -1490,7 +1473,7 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1504,15 +1487,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G2" s="2" t="s">
@@ -1527,7 +1510,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>4</v>
@@ -1548,28 +1531,28 @@
         <v>1</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="38"/>
+      <c r="G4" s="42"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="10"/>
       <c r="C5" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="39"/>
+      <c r="G5" s="43"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
@@ -1578,24 +1561,24 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="39"/>
+      <c r="G6" s="43"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
         <v>2</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="39"/>
+      <c r="G7" s="43"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
@@ -1604,20 +1587,20 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="40"/>
+      <c r="G8" s="44"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>3</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -1640,7 +1623,7 @@
         <v>23</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="1"/>
@@ -1651,7 +1634,7 @@
       <c r="A12" s="16"/>
       <c r="B12" s="15"/>
       <c r="C12" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D12" s="28"/>
       <c r="E12" s="1"/>
@@ -1661,9 +1644,7 @@
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
       <c r="B13" s="15"/>
-      <c r="C13" s="23" t="s">
-        <v>49</v>
-      </c>
+      <c r="C13" s="23"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>

</xml_diff>

<commit_message>
-Update layout for service table
</commit_message>
<xml_diff>
--- a/document/Task_Planning.xlsx
+++ b/document/Task_Planning.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Phuc" sheetId="7" r:id="rId2"/>
     <sheet name="Pending" sheetId="6" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" calcMode="manual" calcCompleted="0"/>
+  <calcPr calcId="152511" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
   <si>
     <t>Accounting</t>
   </si>
@@ -151,15 +151,6 @@
     <t>Default chỉ hiện các job chưa xử lý</t>
   </si>
   <si>
-    <t>Manifest</t>
-  </si>
-  <si>
-    <t>FCL/LCL</t>
-  </si>
-  <si>
-    <t>Khi chuyển đổi -&gt; ảnh hưởng trucking</t>
-  </si>
-  <si>
     <t>JS tính tổng tiền tạm ứng</t>
   </si>
   <si>
@@ -188,6 +179,9 @@
   </si>
   <si>
     <t>Vietnamese for all English terms</t>
+  </si>
+  <si>
+    <t>Sửa lại template bảng báo giá</t>
   </si>
 </sst>
 </file>
@@ -367,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -440,6 +434,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -461,9 +458,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -747,7 +742,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,21 +756,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G2" s="2"/>
       <c r="H2">
         <f>SUM(H4:H41)</f>
-        <v>2350</v>
+        <v>2400</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -815,11 +810,11 @@
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="45">
+      <c r="G4" s="38">
         <v>42102</v>
       </c>
       <c r="H4" s="1">
@@ -833,11 +828,11 @@
         <v>9</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="45">
+      <c r="G5" s="38">
         <v>42102</v>
       </c>
       <c r="H5" s="1">
@@ -851,15 +846,15 @@
         <v>10</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="45">
+      <c r="G6" s="38">
         <v>42102</v>
       </c>
       <c r="H6" s="1">
-        <v>250</v>
+        <v>300</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -869,11 +864,11 @@
         <v>11</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="45">
+      <c r="G7" s="38">
         <v>42105</v>
       </c>
       <c r="H7" s="1">
@@ -887,11 +882,11 @@
         <v>18</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="45">
+      <c r="G8" s="38">
         <v>42103</v>
       </c>
       <c r="H8" s="1">
@@ -912,7 +907,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="39">
+      <c r="H9" s="40">
         <v>250</v>
       </c>
     </row>
@@ -926,7 +921,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="40"/>
+      <c r="H10" s="41"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
@@ -938,7 +933,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="41"/>
+      <c r="H11" s="42"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
@@ -974,7 +969,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="29"/>
-      <c r="H13" s="39">
+      <c r="H13" s="40">
         <v>500</v>
       </c>
     </row>
@@ -988,7 +983,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="29"/>
-      <c r="H14" s="40"/>
+      <c r="H14" s="41"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
@@ -1000,7 +995,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="29"/>
-      <c r="H15" s="40"/>
+      <c r="H15" s="41"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
@@ -1012,7 +1007,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="29"/>
-      <c r="H16" s="41"/>
+      <c r="H16" s="42"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
@@ -1054,10 +1049,10 @@
       <c r="A19" s="9"/>
       <c r="B19" s="17"/>
       <c r="C19" s="25" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -1172,7 +1167,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1186,16 +1181,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G2" s="2" t="s">
@@ -1287,7 +1282,7 @@
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
       <c r="B7" s="17"/>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="46" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="1"/>
@@ -1324,7 +1319,7 @@
         <v>34</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1342,7 +1337,7 @@
         <v>36</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1356,7 +1351,7 @@
       <c r="A11" s="9"/>
       <c r="B11" s="17"/>
       <c r="C11" s="35" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D11" s="36"/>
       <c r="E11" s="36"/>
@@ -1473,7 +1468,7 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1487,15 +1482,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G2" s="2" t="s">
@@ -1541,7 +1536,7 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="42"/>
+      <c r="G4" s="43"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
@@ -1552,7 +1547,7 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="43"/>
+      <c r="G5" s="44"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
@@ -1561,7 +1556,7 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="43"/>
+      <c r="G6" s="44"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
@@ -1578,7 +1573,7 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="43"/>
+      <c r="G7" s="44"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
@@ -1587,21 +1582,13 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="44"/>
+      <c r="G8" s="45"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="16">
-        <v>3</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="A9" s="16"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -1623,7 +1610,7 @@
         <v>23</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="1"/>
@@ -1634,7 +1621,7 @@
       <c r="A12" s="16"/>
       <c r="B12" s="15"/>
       <c r="C12" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D12" s="28"/>
       <c r="E12" s="1"/>
@@ -1644,7 +1631,9 @@
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
       <c r="B13" s="15"/>
-      <c r="C13" s="23"/>
+      <c r="C13" s="23" t="s">
+        <v>51</v>
+      </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>

</xml_diff>

<commit_message>
- update exhibition report
</commit_message>
<xml_diff>
--- a/document/Task_Planning.xlsx
+++ b/document/Task_Planning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Hien" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="67">
   <si>
     <t>Accounting</t>
   </si>
@@ -139,9 +139,6 @@
   </si>
   <si>
     <t>Filters</t>
-  </si>
-  <si>
-    <t>UI decoration</t>
   </si>
   <si>
     <t>Sales</t>
@@ -262,6 +259,12 @@
   </si>
   <si>
     <t>Open</t>
+  </si>
+  <si>
+    <t>Vietnamese</t>
+  </si>
+  <si>
+    <t>Update new request</t>
   </si>
 </sst>
 </file>
@@ -846,8 +849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -915,7 +918,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="44" t="s">
@@ -933,7 +936,7 @@
         <v>9</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
@@ -951,11 +954,13 @@
         <v>10</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="1"/>
+        <v>43</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="F6" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G6" s="38"/>
       <c r="H6" s="1">
@@ -969,7 +974,7 @@
         <v>11</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -985,7 +990,7 @@
         <v>18</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -1148,14 +1153,14 @@
       <c r="A19" s="9"/>
       <c r="B19" s="17"/>
       <c r="C19" s="25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G19" s="29"/>
       <c r="H19" s="1">
@@ -1283,7 +1288,7 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>2</v>
@@ -1292,10 +1297,10 @@
         <v>3</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>56</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>57</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>1</v>
@@ -1306,19 +1311,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D3" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="F3" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1484,7 +1489,7 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>2</v>
@@ -1493,10 +1498,10 @@
         <v>3</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>56</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>57</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>1</v>
@@ -1507,19 +1512,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D3" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="F3" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1826,7 +1831,7 @@
         <v>34</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1846,12 +1851,12 @@
         <v>36</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="33">
@@ -1862,7 +1867,7 @@
       <c r="A11" s="9"/>
       <c r="B11" s="17"/>
       <c r="C11" s="35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D11" s="43"/>
       <c r="E11" s="36"/>
@@ -1980,8 +1985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2045,7 +2050,7 @@
         <v>36</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -2055,7 +2060,7 @@
       <c r="A5" s="16"/>
       <c r="B5" s="10"/>
       <c r="C5" s="1" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -2076,13 +2081,13 @@
         <v>2</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -2123,7 +2128,7 @@
         <v>23</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="1"/>
@@ -2134,7 +2139,7 @@
       <c r="A12" s="16"/>
       <c r="B12" s="15"/>
       <c r="C12" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" s="28"/>
       <c r="E12" s="1"/>
@@ -2145,7 +2150,7 @@
       <c r="A13" s="16"/>
       <c r="B13" s="15"/>
       <c r="C13" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>

</xml_diff>

<commit_message>
Finish bang ke nha thau
</commit_message>
<xml_diff>
--- a/document/Task_Planning.xlsx
+++ b/document/Task_Planning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Hien" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="81">
   <si>
     <t>Accounting</t>
   </si>
@@ -304,6 +304,9 @@
   </si>
   <si>
     <t>20/4</t>
+  </si>
+  <si>
+    <t>Done by Linh</t>
   </si>
 </sst>
 </file>
@@ -573,31 +576,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -881,8 +884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,21 +899,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G2" s="2"/>
       <c r="H2">
         <f>SUM(H4:H41)</f>
-        <v>2250</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1025,11 +1028,11 @@
         <v>40</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="G8" s="35"/>
-      <c r="H8" s="1">
-        <v>150</v>
-      </c>
+      <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
@@ -1043,11 +1046,11 @@
       </c>
       <c r="D9" s="13"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="47" t="s">
+      <c r="F9" s="50" t="s">
         <v>31</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="44">
+      <c r="H9" s="47">
         <v>50</v>
       </c>
     </row>
@@ -1059,9 +1062,9 @@
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="48"/>
+      <c r="F10" s="51"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="45"/>
+      <c r="H10" s="48"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
@@ -1071,9 +1074,9 @@
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="49"/>
+      <c r="F11" s="52"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="46"/>
+      <c r="H11" s="49"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
@@ -1111,7 +1114,7 @@
         <v>31</v>
       </c>
       <c r="G13" s="26"/>
-      <c r="H13" s="44">
+      <c r="H13" s="47">
         <v>500</v>
       </c>
     </row>
@@ -1125,7 +1128,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="26"/>
-      <c r="H14" s="45"/>
+      <c r="H14" s="48"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
@@ -1137,7 +1140,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="26"/>
-      <c r="H15" s="45"/>
+      <c r="H15" s="48"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
@@ -1149,7 +1152,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="26"/>
-      <c r="H16" s="46"/>
+      <c r="H16" s="49"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
@@ -1733,16 +1736,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G2" s="2" t="s">
@@ -2027,8 +2030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2043,15 +2046,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G2" s="2" t="s">
@@ -2080,7 +2083,7 @@
       <c r="G3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="52"/>
+      <c r="J3" s="45"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
@@ -2111,7 +2114,9 @@
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="G5" s="13" t="s">
         <v>76</v>
       </c>
@@ -2124,7 +2129,9 @@
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="G6" s="13" t="s">
         <v>76</v>
       </c>
@@ -2137,7 +2144,9 @@
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="G7" s="13" t="s">
         <v>76</v>
       </c>
@@ -2145,12 +2154,14 @@
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
       <c r="B8" s="17"/>
-      <c r="C8" s="50" t="s">
+      <c r="C8" s="43" t="s">
         <v>66</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="G8" s="13" t="s">
         <v>76</v>
       </c>
@@ -2158,7 +2169,7 @@
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="10"/>
-      <c r="C9" s="50" t="s">
+      <c r="C9" s="43" t="s">
         <v>68</v>
       </c>
       <c r="D9" s="1"/>
@@ -2208,21 +2219,26 @@
       <c r="E12" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="G12" s="50" t="s">
+      <c r="F12" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="43" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
       <c r="B13" s="15"/>
-      <c r="C13" s="51" t="s">
+      <c r="C13" s="44" t="s">
         <v>71</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F13" s="1"/>
+      <c r="F13" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="G13" s="1" t="s">
         <v>76</v>
       </c>
@@ -2241,7 +2257,9 @@
       <c r="E14" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F14" s="1"/>
+      <c r="F14" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="G14" s="1" t="s">
         <v>76</v>
       </c>
@@ -2267,7 +2285,9 @@
       <c r="E16" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F16" s="1"/>
+      <c r="F16" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="G16" s="23" t="s">
         <v>76</v>
       </c>
@@ -2295,7 +2315,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update bug tam ung
</commit_message>
<xml_diff>
--- a/document/Task_Planning.xlsx
+++ b/document/Task_Planning.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="90">
   <si>
     <t>Accounting</t>
   </si>
@@ -331,6 +331,9 @@
   </si>
   <si>
     <t>Chưa tính tổng cho tồn tạm ứng</t>
+  </si>
+  <si>
+    <t>Chọn ngày mặc định cho ngày tạm ứng là current date, mặt đình cho ngày hoàn ứng là 1 tháng sau</t>
   </si>
 </sst>
 </file>
@@ -1341,7 +1344,7 @@
   <dimension ref="A2:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1441,14 +1444,16 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
+      <c r="E7" s="42" t="s">
+        <v>89</v>
+      </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add template cho thong quan (ke hoach van tai)
</commit_message>
<xml_diff>
--- a/document/Task_Planning.xlsx
+++ b/document/Task_Planning.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="95">
   <si>
     <t>Accounting</t>
   </si>
@@ -334,6 +334,21 @@
   </si>
   <si>
     <t>Chọn ngày mặc định cho ngày tạm ứng là current date, mặt đình cho ngày hoàn ứng là 1 tháng sau</t>
+  </si>
+  <si>
+    <t>Tong hop cong no</t>
+  </si>
+  <si>
+    <t>Khi ko chọn ngày default ngày bắt đầu ngày kết thúc là hôm nay</t>
+  </si>
+  <si>
+    <t>Không chọn date</t>
+  </si>
+  <si>
+    <t>Search ok</t>
+  </si>
+  <si>
+    <t>Active tab ko phải là tab công nợ</t>
   </si>
 </sst>
 </file>
@@ -519,7 +534,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -628,6 +643,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1344,7 +1362,7 @@
   <dimension ref="A2:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1456,14 +1474,22 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
+      <c r="B8" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="E8" s="42" t="s">
+        <v>91</v>
+      </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1472,8 +1498,12 @@
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
+      <c r="D9" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="E9" s="42" t="s">
+        <v>94</v>
+      </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2082,7 +2112,7 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2353,7 +2383,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -2366,7 +2396,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Done ke hoach van tai report cho thong quan
</commit_message>
<xml_diff>
--- a/document/Task_Planning.xlsx
+++ b/document/Task_Planning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Hien" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="97">
   <si>
     <t>Accounting</t>
   </si>
@@ -349,6 +349,12 @@
   </si>
   <si>
     <t>Active tab ko phải là tab công nợ</t>
+  </si>
+  <si>
+    <t>Tong hop cong no nhan vien</t>
+  </si>
+  <si>
+    <t>Ở page nhân viên, ko cho xem của người khác</t>
   </si>
 </sst>
 </file>
@@ -623,6 +629,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -643,9 +652,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -944,15 +950,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G2" s="2"/>
@@ -1091,11 +1097,11 @@
       </c>
       <c r="D9" s="13"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="50" t="s">
+      <c r="F9" s="51" t="s">
         <v>31</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="47">
+      <c r="H9" s="48">
         <v>50</v>
       </c>
     </row>
@@ -1107,9 +1113,9 @@
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="51"/>
+      <c r="F10" s="52"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="48"/>
+      <c r="H10" s="49"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
@@ -1119,9 +1125,9 @@
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="52"/>
+      <c r="F11" s="53"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="49"/>
+      <c r="H11" s="50"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
@@ -1159,7 +1165,7 @@
         <v>31</v>
       </c>
       <c r="G13" s="26"/>
-      <c r="H13" s="47">
+      <c r="H13" s="48">
         <v>500</v>
       </c>
     </row>
@@ -1175,7 +1181,7 @@
         <v>31</v>
       </c>
       <c r="G14" s="26"/>
-      <c r="H14" s="48"/>
+      <c r="H14" s="49"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
@@ -1189,7 +1195,7 @@
         <v>31</v>
       </c>
       <c r="G15" s="26"/>
-      <c r="H15" s="48"/>
+      <c r="H15" s="49"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
@@ -1203,7 +1209,7 @@
         <v>31</v>
       </c>
       <c r="G16" s="26"/>
-      <c r="H16" s="49"/>
+      <c r="H16" s="50"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
@@ -1361,8 +1367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1484,7 +1490,7 @@
       <c r="C8" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="53" t="s">
+      <c r="D8" s="46" t="s">
         <v>92</v>
       </c>
       <c r="E8" s="42" t="s">
@@ -1506,14 +1512,18 @@
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
+      <c r="D10" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" s="42" t="s">
+        <v>96</v>
+      </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1817,16 +1827,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G2" s="2" t="s">
@@ -2111,8 +2121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2127,15 +2137,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G2" s="2" t="s">
@@ -2407,7 +2417,9 @@
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+      <c r="F19" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="G19" s="1" t="s">
         <v>79</v>
       </c>

</xml_diff>

<commit_message>
- Prepare for test version 22042015
</commit_message>
<xml_diff>
--- a/document/Task_Planning.xlsx
+++ b/document/Task_Planning.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="97">
   <si>
     <t>Accounting</t>
   </si>
@@ -2122,7 +2122,7 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2391,7 +2391,9 @@
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+      <c r="F17" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="G17" s="1" t="s">
         <v>79</v>
       </c>
@@ -2404,7 +2406,9 @@
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="F18" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="G18" s="1" t="s">
         <v>79</v>
       </c>

</xml_diff>

<commit_message>
fix tam ung bug
</commit_message>
<xml_diff>
--- a/document/Task_Planning.xlsx
+++ b/document/Task_Planning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hien" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="102">
   <si>
     <t>Accounting</t>
   </si>
@@ -355,6 +355,21 @@
   </si>
   <si>
     <t>Ở page nhân viên, ko cho xem của người khác</t>
+  </si>
+  <si>
+    <t>Button layout ko chính xác</t>
+  </si>
+  <si>
+    <t>Ton tam ung</t>
+  </si>
+  <si>
+    <t>Chi tinh ton tam ung cua cung nguoi dùng va cùng job</t>
+  </si>
+  <si>
+    <t>Load ton tam ung cho row khi add va khi change</t>
+  </si>
+  <si>
+    <t>Ton tam ung bi NaN khi nhập số từ hàng ngàn</t>
   </si>
 </sst>
 </file>
@@ -1367,8 +1382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1393,9 +1408,6 @@
       <c r="D2" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="18" t="s">
-        <v>51</v>
-      </c>
       <c r="F2" s="18" t="s">
         <v>1</v>
       </c>
@@ -1526,44 +1538,58 @@
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="42"/>
+      <c r="B11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>97</v>
+      </c>
       <c r="E11" s="42"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
+      <c r="E12" s="42" t="s">
+        <v>99</v>
+      </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
+      <c r="E13" s="42" t="s">
+        <v>100</v>
+      </c>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
+      <c r="E14" s="42" t="s">
+        <v>101</v>
+      </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2121,7 +2147,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add bo phan cho phieu de nghi thanh toan
</commit_message>
<xml_diff>
--- a/document/Task_Planning.xlsx
+++ b/document/Task_Planning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Hien" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="103">
   <si>
     <t>Accounting</t>
   </si>
@@ -163,12 +163,6 @@
   </si>
   <si>
     <t>Vietnamese for all English terms</t>
-  </si>
-  <si>
-    <t>Pending</t>
-  </si>
-  <si>
-    <t>In Progress</t>
   </si>
   <si>
     <t>Modification</t>
@@ -370,6 +364,15 @@
   </si>
   <si>
     <t>Ton tam ung bi NaN khi nhập số từ hàng ngàn</t>
+  </si>
+  <si>
+    <t>Done by Hien</t>
+  </si>
+  <si>
+    <t>update giá, chỉ select ko có layout</t>
+  </si>
+  <si>
+    <t>Bonus</t>
   </si>
 </sst>
 </file>
@@ -950,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,8 +981,8 @@
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G2" s="2"/>
       <c r="H2">
-        <f>SUM(H4:H41)</f>
-        <v>2100</v>
+        <f>SUM(H4:H19)</f>
+        <v>1500</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1058,10 +1061,10 @@
         <v>39</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="G6" s="35"/>
       <c r="H6" s="1">
@@ -1078,11 +1081,11 @@
         <v>40</v>
       </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="G7" s="35"/>
-      <c r="H7" s="1">
-        <v>300</v>
-      </c>
+      <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
@@ -1095,7 +1098,7 @@
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G8" s="35"/>
       <c r="H8" s="1"/>
@@ -1181,7 +1184,7 @@
       </c>
       <c r="G13" s="26"/>
       <c r="H13" s="48">
-        <v>500</v>
+        <v>600</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1238,11 +1241,11 @@
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+      <c r="F17" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="G17" s="26"/>
-      <c r="H17" s="1">
-        <v>300</v>
-      </c>
+      <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
@@ -1252,11 +1255,11 @@
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="F18" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="G18" s="26"/>
-      <c r="H18" s="1">
-        <v>100</v>
-      </c>
+      <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
@@ -1265,11 +1268,11 @@
         <v>41</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="G19" s="26"/>
       <c r="H19" s="1">
@@ -1283,10 +1286,23 @@
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="5"/>
+      <c r="F21" t="s">
+        <v>102</v>
+      </c>
+      <c r="H21">
+        <v>1000</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="5"/>
+      <c r="F22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22">
+        <f>H2+H21</f>
+        <v>2500</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
@@ -1382,7 +1398,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -1397,7 +1413,7 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>2</v>
@@ -1406,7 +1422,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>1</v>
@@ -1417,19 +1433,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D3" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="E3" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1437,16 +1453,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D4" s="42" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E4" s="42" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F4" s="1"/>
     </row>
@@ -1455,16 +1471,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="42" t="s">
         <v>84</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="E5" s="42" t="s">
-        <v>86</v>
       </c>
       <c r="F5" s="1"/>
     </row>
@@ -1476,7 +1492,7 @@
       <c r="C6" s="1"/>
       <c r="D6" s="42"/>
       <c r="E6" s="42" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F6" s="1"/>
     </row>
@@ -1488,7 +1504,7 @@
       <c r="C7" s="1"/>
       <c r="D7" s="42"/>
       <c r="E7" s="42" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F7" s="1"/>
     </row>
@@ -1497,16 +1513,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D8" s="46" t="s">
-        <v>92</v>
-      </c>
       <c r="E8" s="42" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F8" s="1"/>
     </row>
@@ -1517,10 +1533,10 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="42" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E9" s="42" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F9" s="1"/>
     </row>
@@ -1531,10 +1547,10 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="42" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E10" s="42" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F10" s="1"/>
     </row>
@@ -1543,13 +1559,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D11" s="42" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E11" s="42"/>
       <c r="F11" s="1"/>
@@ -1560,11 +1576,11 @@
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D12" s="42"/>
       <c r="E12" s="42" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F12" s="1"/>
     </row>
@@ -1576,7 +1592,7 @@
       <c r="C13" s="1"/>
       <c r="D13" s="42"/>
       <c r="E13" s="42" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F13" s="1"/>
     </row>
@@ -1588,7 +1604,7 @@
       <c r="C14" s="1"/>
       <c r="D14" s="42"/>
       <c r="E14" s="42" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F14" s="1"/>
     </row>
@@ -1645,7 +1661,7 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>2</v>
@@ -1654,10 +1670,10 @@
         <v>3</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>1</v>
@@ -1668,19 +1684,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D3" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="E3" s="42" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1688,13 +1704,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="42" t="s">
         <v>81</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D4" s="42" t="s">
-        <v>83</v>
       </c>
       <c r="E4" s="42"/>
       <c r="F4" s="1"/>
@@ -1836,10 +1852,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1850,9 +1866,10 @@
     <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="47" t="s">
         <v>32</v>
       </c>
@@ -1864,16 +1881,16 @@
       <c r="G1" s="47"/>
       <c r="H1" s="47"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G2" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H2">
-        <f>SUM(H4:H20)</f>
-        <v>2300</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <f ca="1">SUM(H4:H20)</f>
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
@@ -1899,7 +1916,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
         <v>1</v>
       </c>
@@ -1911,15 +1928,20 @@
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="G4" s="26">
         <v>42104</v>
       </c>
       <c r="H4" s="1">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="I4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="14"/>
       <c r="C5" s="20" t="s">
@@ -1934,10 +1956,10 @@
         <v>42102</v>
       </c>
       <c r="H5" s="1">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="10"/>
       <c r="C6" s="22" t="s">
@@ -1947,13 +1969,18 @@
       <c r="E6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="I6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
       <c r="B7" s="17"/>
       <c r="C7" s="36" t="s">
@@ -1961,13 +1988,15 @@
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="19">
         <v>2</v>
       </c>
@@ -1979,13 +2008,13 @@
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>100</v>
+      </c>
       <c r="G8" s="1"/>
-      <c r="H8" s="13">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H8" s="13"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="19">
         <v>3</v>
       </c>
@@ -2005,7 +2034,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="31">
         <v>4</v>
       </c>
@@ -2025,7 +2054,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="17"/>
       <c r="C11" s="32" t="s">
@@ -2033,31 +2062,44 @@
       </c>
       <c r="D11" s="40"/>
       <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
+      <c r="F11" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="G11" s="33"/>
-      <c r="H11" s="34">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H11" s="34"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="37"/>
       <c r="C12" s="38"/>
       <c r="D12" s="39"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="5"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>102</v>
+      </c>
+      <c r="H13">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14">
+        <f ca="1">H2+H13</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="5"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="5"/>
     </row>
@@ -2148,7 +2190,7 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2227,7 +2269,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -2235,14 +2277,14 @@
         <v>31</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
       <c r="B6" s="10"/>
       <c r="C6" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -2250,14 +2292,14 @@
         <v>31</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="10"/>
       <c r="C7" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -2265,14 +2307,14 @@
         <v>31</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
       <c r="B8" s="17"/>
       <c r="C8" s="43" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -2280,33 +2322,37 @@
         <v>31</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="10"/>
       <c r="C9" s="43" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="G9" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
       <c r="B10" s="17"/>
       <c r="C10" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="G10" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -2314,7 +2360,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C11" s="22"/>
       <c r="D11" s="23"/>
@@ -2327,37 +2373,37 @@
         <v>4</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F12" t="s">
         <v>31</v>
       </c>
       <c r="G12" s="43" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
       <c r="B13" s="15"/>
       <c r="C13" s="44" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>31</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2368,24 +2414,24 @@
         <v>0</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>31</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="10"/>
       <c r="C15" s="21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -2396,17 +2442,17 @@
       <c r="A16" s="9"/>
       <c r="B16" s="17"/>
       <c r="C16" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>31</v>
       </c>
       <c r="G16" s="23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2418,17 +2464,17 @@
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="17"/>
       <c r="C18" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -2436,7 +2482,7 @@
         <v>31</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -2451,7 +2497,7 @@
         <v>31</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
- Update profit loss
</commit_message>
<xml_diff>
--- a/document/Task_Planning.xlsx
+++ b/document/Task_Planning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hien" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="120">
   <si>
     <t>Accounting</t>
   </si>
@@ -409,6 +409,21 @@
   </si>
   <si>
     <t>reuse page thanh toán</t>
+  </si>
+  <si>
+    <t>Ke hoach van tai</t>
+  </si>
+  <si>
+    <t>Nha thau</t>
+  </si>
+  <si>
+    <t>Select job ko cho select job thông quan/exh ở phần vận tải và tương tự cho thông quan</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Đổi tên label cho phù hợp</t>
   </si>
 </sst>
 </file>
@@ -675,6 +690,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -696,7 +712,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -979,8 +994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,15 +1009,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G2" s="2"/>
@@ -1141,11 +1156,11 @@
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="50" t="s">
+      <c r="F9" s="51" t="s">
         <v>31</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="47">
+      <c r="H9" s="48">
         <v>50</v>
       </c>
     </row>
@@ -1157,9 +1172,9 @@
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="51"/>
+      <c r="F10" s="52"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="48"/>
+      <c r="H10" s="49"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
@@ -1169,9 +1184,9 @@
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="52"/>
+      <c r="F11" s="53"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="49"/>
+      <c r="H11" s="50"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
@@ -1209,7 +1224,7 @@
         <v>31</v>
       </c>
       <c r="G13" s="25"/>
-      <c r="H13" s="47">
+      <c r="H13" s="48">
         <v>600</v>
       </c>
     </row>
@@ -1225,7 +1240,7 @@
         <v>31</v>
       </c>
       <c r="G14" s="25"/>
-      <c r="H14" s="48"/>
+      <c r="H14" s="49"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
@@ -1239,7 +1254,7 @@
         <v>31</v>
       </c>
       <c r="G15" s="25"/>
-      <c r="H15" s="48"/>
+      <c r="H15" s="49"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
@@ -1253,7 +1268,7 @@
         <v>31</v>
       </c>
       <c r="G16" s="25"/>
-      <c r="H16" s="49"/>
+      <c r="H16" s="50"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="18">
@@ -1310,7 +1325,7 @@
         <v>6</v>
       </c>
       <c r="B20" s="16"/>
-      <c r="C20" s="53" t="s">
+      <c r="C20" s="46" t="s">
         <v>113</v>
       </c>
       <c r="D20" s="1"/>
@@ -1426,8 +1441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F18"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1572,7 +1587,9 @@
       <c r="E9" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -1703,8 +1720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1752,7 +1769,7 @@
         <v>51</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1769,7 +1786,9 @@
         <v>81</v>
       </c>
       <c r="E4" s="41"/>
-      <c r="F4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -1785,7 +1804,9 @@
       <c r="E5" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -1799,25 +1820,39 @@
       <c r="E6" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>115</v>
+      </c>
       <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
+      <c r="E7" s="41" t="s">
+        <v>117</v>
+      </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="41"/>
+      <c r="B8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D8" s="41" t="s">
+        <v>119</v>
+      </c>
       <c r="E8" s="41"/>
       <c r="F8" s="1"/>
     </row>
@@ -1936,16 +1971,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G2" s="2" t="s">
@@ -2264,15 +2299,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G2" s="2" t="s">

</xml_diff>

<commit_message>
- Create TinhNangHeThong - 1st Release version
</commit_message>
<xml_diff>
--- a/document/Task_Planning.xlsx
+++ b/document/Task_Planning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Hien" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Phuc" sheetId="7" r:id="rId4"/>
     <sheet name="Pending" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511" calcMode="manual"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="122">
   <si>
     <t>Accounting</t>
   </si>
@@ -424,6 +424,12 @@
   </si>
   <si>
     <t>Đổi tên label cho phù hợp</t>
+  </si>
+  <si>
+    <t>Ton tam ung chua xet ngay thang</t>
+  </si>
+  <si>
+    <t>Refund Job</t>
   </si>
 </sst>
 </file>
@@ -601,7 +607,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -673,7 +679,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -712,6 +717,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -994,7 +1001,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -1009,15 +1016,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G2" s="2"/>
@@ -1066,7 +1073,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="40" t="s">
+      <c r="F4" s="39" t="s">
         <v>31</v>
       </c>
       <c r="G4" s="34"/>
@@ -1156,11 +1163,11 @@
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="51" t="s">
+      <c r="F9" s="50" t="s">
         <v>31</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="48">
+      <c r="H9" s="47">
         <v>50</v>
       </c>
     </row>
@@ -1172,9 +1179,9 @@
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="52"/>
+      <c r="F10" s="51"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="49"/>
+      <c r="H10" s="48"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
@@ -1184,9 +1191,9 @@
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="53"/>
+      <c r="F11" s="52"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="50"/>
+      <c r="H11" s="49"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
@@ -1224,7 +1231,7 @@
         <v>31</v>
       </c>
       <c r="G13" s="25"/>
-      <c r="H13" s="48">
+      <c r="H13" s="47">
         <v>600</v>
       </c>
     </row>
@@ -1240,7 +1247,7 @@
         <v>31</v>
       </c>
       <c r="G14" s="25"/>
-      <c r="H14" s="49"/>
+      <c r="H14" s="48"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
@@ -1254,7 +1261,7 @@
         <v>31</v>
       </c>
       <c r="G15" s="25"/>
-      <c r="H15" s="49"/>
+      <c r="H15" s="48"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
@@ -1268,7 +1275,7 @@
         <v>31</v>
       </c>
       <c r="G16" s="25"/>
-      <c r="H16" s="50"/>
+      <c r="H16" s="49"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="18">
@@ -1325,7 +1332,7 @@
         <v>6</v>
       </c>
       <c r="B20" s="16"/>
-      <c r="C20" s="46" t="s">
+      <c r="C20" s="45" t="s">
         <v>113</v>
       </c>
       <c r="D20" s="1"/>
@@ -1439,10 +1446,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F18"/>
+  <dimension ref="A2:F19"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1481,10 +1488,10 @@
       <c r="C3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="40" t="s">
         <v>56</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -1501,10 +1508,10 @@
       <c r="C4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="41" t="s">
+      <c r="E4" s="40" t="s">
         <v>60</v>
       </c>
       <c r="F4" s="1"/>
@@ -1519,10 +1526,10 @@
       <c r="C5" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="D5" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="40" t="s">
         <v>84</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -1535,8 +1542,8 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41" t="s">
+      <c r="D6" s="40"/>
+      <c r="E6" s="40" t="s">
         <v>86</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -1549,8 +1556,8 @@
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41" t="s">
+      <c r="D7" s="40"/>
+      <c r="E7" s="40" t="s">
         <v>87</v>
       </c>
       <c r="F7" s="1"/>
@@ -1565,10 +1572,10 @@
       <c r="C8" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D8" s="45" t="s">
+      <c r="D8" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="E8" s="41" t="s">
+      <c r="E8" s="40" t="s">
         <v>89</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -1581,10 +1588,10 @@
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="41" t="s">
+      <c r="D9" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="E9" s="41" t="s">
+      <c r="E9" s="40" t="s">
         <v>92</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -1597,10 +1604,10 @@
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="41" t="s">
+      <c r="D10" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="E10" s="41" t="s">
+      <c r="E10" s="40" t="s">
         <v>94</v>
       </c>
       <c r="F10" s="1"/>
@@ -1615,10 +1622,10 @@
       <c r="C11" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D11" s="41" t="s">
+      <c r="D11" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="E11" s="41"/>
+      <c r="E11" s="40"/>
       <c r="F11" s="1" t="s">
         <v>31</v>
       </c>
@@ -1631,8 +1638,8 @@
       <c r="C12" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41" t="s">
+      <c r="D12" s="40"/>
+      <c r="E12" s="40" t="s">
         <v>97</v>
       </c>
       <c r="F12" s="1" t="s">
@@ -1645,8 +1652,8 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41" t="s">
+      <c r="D13" s="40"/>
+      <c r="E13" s="40" t="s">
         <v>98</v>
       </c>
       <c r="F13" s="1"/>
@@ -1657,8 +1664,8 @@
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41" t="s">
+      <c r="D14" s="40"/>
+      <c r="E14" s="40" t="s">
         <v>99</v>
       </c>
       <c r="F14" s="1"/>
@@ -1671,8 +1678,8 @@
       <c r="C15" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41" t="s">
+      <c r="D15" s="40"/>
+      <c r="E15" s="40" t="s">
         <v>103</v>
       </c>
       <c r="F15" s="1"/>
@@ -1683,8 +1690,8 @@
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41" t="s">
+      <c r="D16" s="40"/>
+      <c r="E16" s="40" t="s">
         <v>108</v>
       </c>
       <c r="F16" s="1"/>
@@ -1695,8 +1702,8 @@
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41" t="s">
+      <c r="D17" s="40"/>
+      <c r="E17" s="40" t="s">
         <v>109</v>
       </c>
       <c r="F17" s="1" t="s">
@@ -1704,11 +1711,16 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E18" s="45" t="s">
+      <c r="E18" s="44" t="s">
         <v>110</v>
       </c>
       <c r="F18" t="s">
         <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E19" s="44" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1720,8 +1732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1762,10 +1774,10 @@
       <c r="C3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="40" t="s">
         <v>51</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -1782,10 +1794,10 @@
       <c r="C4" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="E4" s="41"/>
+      <c r="E4" s="40"/>
       <c r="F4" s="1" t="s">
         <v>31</v>
       </c>
@@ -1800,8 +1812,8 @@
       <c r="C5" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41" t="s">
+      <c r="D5" s="40"/>
+      <c r="E5" s="40" t="s">
         <v>106</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -1816,8 +1828,8 @@
         <v>82</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41" t="s">
+      <c r="D6" s="40"/>
+      <c r="E6" s="40" t="s">
         <v>107</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -1834,8 +1846,8 @@
       <c r="C7" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41" t="s">
+      <c r="D7" s="40"/>
+      <c r="E7" s="40" t="s">
         <v>117</v>
       </c>
       <c r="F7" s="1"/>
@@ -1850,10 +1862,10 @@
       <c r="C8" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D8" s="41" t="s">
+      <c r="D8" s="40" t="s">
         <v>119</v>
       </c>
-      <c r="E8" s="41"/>
+      <c r="E8" s="40"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1862,8 +1874,8 @@
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1872,8 +1884,8 @@
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1882,8 +1894,8 @@
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1892,8 +1904,8 @@
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1902,8 +1914,8 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1912,8 +1924,8 @@
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1922,8 +1934,8 @@
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1932,8 +1944,8 @@
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1942,8 +1954,8 @@
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
       <c r="F17" s="1"/>
     </row>
   </sheetData>
@@ -1955,8 +1967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1971,16 +1983,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G2" s="2" t="s">
@@ -1988,7 +2000,7 @@
       </c>
       <c r="H2">
         <f>SUM(H4:H20)</f>
-        <v>1350</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2029,7 +2041,7 @@
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="40" t="s">
+      <c r="F4" s="39" t="s">
         <v>31</v>
       </c>
       <c r="G4" s="25">
@@ -2161,7 +2173,7 @@
       <c r="C11" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="39"/>
+      <c r="D11" s="38"/>
       <c r="E11" s="32"/>
       <c r="F11" s="1" t="s">
         <v>78</v>
@@ -2172,8 +2184,13 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="36"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="38"/>
+      <c r="C12" s="53" t="s">
+        <v>121</v>
+      </c>
+      <c r="D12" s="37"/>
+      <c r="H12" s="54">
+        <v>200</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
@@ -2299,15 +2316,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G2" s="2" t="s">
@@ -2336,7 +2353,7 @@
       <c r="G3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="44"/>
+      <c r="J3" s="43"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
@@ -2407,7 +2424,7 @@
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
       <c r="B8" s="16"/>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="41" t="s">
         <v>64</v>
       </c>
       <c r="D8" s="1"/>
@@ -2422,7 +2439,7 @@
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
       <c r="B9" s="9"/>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="41" t="s">
         <v>66</v>
       </c>
       <c r="D9" s="1"/>
@@ -2479,14 +2496,14 @@
       <c r="F12" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="42" t="s">
+      <c r="G12" s="41" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
       <c r="B13" s="14"/>
-      <c r="C13" s="43" t="s">
+      <c r="C13" s="42" t="s">
         <v>69</v>
       </c>
       <c r="D13" s="1"/>

</xml_diff>